<commit_message>
Update report template add columns
</commit_message>
<xml_diff>
--- a/TFSBuildUtils/TFSBuildUtils/Build_Report.xlsx
+++ b/TFSBuildUtils/TFSBuildUtils/Build_Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naruto\source\repos\TFSBuildUtils\TFSBuildUtils\TFSBuildUtils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PhongBV\source\repos\TFSBuildUtils\TFSBuildUtils\TFSBuildUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE8A3EE-534D-475A-85BB-1021DF8A22F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E013966C-2ABE-42B3-9F3F-14A9D3304C52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Title</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Area Path</t>
   </si>
   <si>
-    <t>Handle By</t>
-  </si>
-  <si>
     <t>Assign To Tester</t>
   </si>
   <si>
@@ -49,6 +46,12 @@
   </si>
   <si>
     <t>WorkItem ID</t>
+  </si>
+  <si>
+    <t>Build Date</t>
+  </si>
+  <si>
+    <t>Work item type</t>
   </si>
 </sst>
 </file>
@@ -110,10 +113,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -395,47 +398,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="96.5703125" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13" style="2" customWidth="1"/>
+    <col min="5" max="5" width="96.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>